<commit_message>
updated testing report (current to 27/03)
</commit_message>
<xml_diff>
--- a/docs/TestingReport.xlsx
+++ b/docs/TestingReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patch\Desktop\projects\uniProjects\COSC310\the-project-homebase\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\COSC310\the-project-homebase\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF140297-416F-4570-93BD-7D3DFABACBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC75923-4D82-4916-AB90-410BA75CA484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{DB730603-D2D5-4301-96DB-FBA18085EEBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DB730603-D2D5-4301-96DB-FBA18085EEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <r>
       <t xml:space="preserve">Pass or Fail
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>US, UN</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
@@ -473,6 +485,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,12 +499,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,25 +816,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D03DFF-1B5A-497A-B5AA-FDCB6A8C5BF6}">
   <dimension ref="A3:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1328125" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="105" customWidth="1"/>
-    <col min="3" max="3" width="48.59765625" customWidth="1"/>
-    <col min="4" max="4" width="17.796875" customWidth="1"/>
-    <col min="5" max="5" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="4" spans="1:5" ht="103.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="12" t="s">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" ht="103.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="6" t="s">
         <v>31</v>
       </c>
@@ -833,411 +845,431 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D11" s="12"/>
+      <c r="E11" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D12" s="12"/>
+      <c r="E12" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D13" s="12"/>
+      <c r="E13" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D14" s="12"/>
+      <c r="E14" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D15" s="12"/>
+      <c r="E15" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>11.1</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>11.2</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>11.3</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>11.4</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D21" s="12"/>
+      <c r="E21" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D22" s="12"/>
+      <c r="E22" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>14</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D23" s="12"/>
+      <c r="E23" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>14.1</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D24" s="12"/>
+      <c r="E24" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>14.2</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D25" s="12"/>
+      <c r="E25" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>14.3</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D26" s="12"/>
+      <c r="E26" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>15</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D27" s="12"/>
+      <c r="E27" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>16</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="14" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D30" s="12"/>
+      <c r="E30" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D31" s="12"/>
+      <c r="E31" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="13" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>